<commit_message>
correction of cosine measure + analyze_results.py
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="89">
   <si>
     <t>dfadfaa39598cf760125439346d903ea0467e7fa</t>
   </si>
@@ -284,6 +285,15 @@
   </si>
   <si>
     <t>SOVHDXE12A6310FF8A</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>hours</t>
   </si>
 </sst>
 </file>
@@ -2053,7 +2063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2759,4 +2769,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2.3741999999999999E-2</v>
+      </c>
+      <c r="B1">
+        <v>110000</v>
+      </c>
+      <c r="C1">
+        <f>B1*A1</f>
+        <v>2611.62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>C1/60</f>
+        <v>43.527000000000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>C2/60</f>
+        <v>0.72545000000000004</v>
+      </c>
+      <c r="D3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0.33333299999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0.103448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f>SUM(H4:H6)</f>
+        <v>0.68678099999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>1/1*(1/24)</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H8">
+        <f>H7/3</f>
+        <v>0.22892699999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>1/(26*4)</f>
+        <v>9.6153846153846159E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>